<commit_message>
Importing KitTemplates from test.xlsx successfuly
</commit_message>
<xml_diff>
--- a/bika/sanbi/setupdata/test/test.xlsx
+++ b/bika/sanbi/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="608" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="758" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,15 +19,17 @@
     <sheet name="Supplier Contacts" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Product Categories" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Products" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Constants" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Stock items" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Stock Items" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Kit Templates" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Kit Components" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Constants" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="650">
   <si>
     <t>Instructions</t>
   </si>
@@ -1082,6 +1084,141 @@
     <t>Humans are subject to nitrate toxicity, with infants being especially vulnerable to methemoglobinemia due to nitrate metabolizing triglycerides present at higher concentrations than at other stages of development. Methemoglobinemia in infants is known as blue baby syndrome. Although nitrates in drinking water were once thought to be a contributing factor, there are now significant scientific doubts as to whether there is a causal link. Blue baby syndrome is now thought to be the product of a number of factors, which can include any factor that causes gastric upset, such as diarrhoeal infection, protein intolerance, heavy metal toxicity etc., with nitrates playing a minor role.</t>
   </si>
   <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>StockItemID</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>labId</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>dateReceived</t>
+  </si>
+  <si>
+    <t>dateOpened</t>
+  </si>
+  <si>
+    <t>expiryDate</t>
+  </si>
+  <si>
+    <t>disposalDate</t>
+  </si>
+  <si>
+    <t>Stock items</t>
+  </si>
+  <si>
+    <t>Stock item ID</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Order Id</t>
+  </si>
+  <si>
+    <t>Lab Id</t>
+  </si>
+  <si>
+    <t>Batch Id</t>
+  </si>
+  <si>
+    <t>Date Received</t>
+  </si>
+  <si>
+    <t>Date Opened</t>
+  </si>
+  <si>
+    <t>Expiry Date</t>
+  </si>
+  <si>
+    <t>Disposal Date</t>
+  </si>
+  <si>
+    <t>id-001</t>
+  </si>
+  <si>
+    <t>test desc</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>id-002</t>
+  </si>
+  <si>
+    <t>id-003</t>
+  </si>
+  <si>
+    <t>id-004</t>
+  </si>
+  <si>
+    <t>id-005</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>id-006</t>
+  </si>
+  <si>
+    <t>id-007</t>
+  </si>
+  <si>
+    <t>id-008</t>
+  </si>
+  <si>
+    <t>id-009</t>
+  </si>
+  <si>
+    <t>templateID</t>
+  </si>
+  <si>
+    <t>templateName</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Kit Templates</t>
+  </si>
+  <si>
+    <t>Template ID</t>
+  </si>
+  <si>
+    <t>Template Name</t>
+  </si>
+  <si>
+    <t>DNA Blood sampling kit</t>
+  </si>
+  <si>
+    <t>RNA Blood sampling kit</t>
+  </si>
+  <si>
+    <t>componentID</t>
+  </si>
+  <si>
+    <t>componentName</t>
+  </si>
+  <si>
+    <t>Component ID</t>
+  </si>
+  <si>
+    <t>Component Name</t>
+  </si>
+  <si>
     <t>AR Import options</t>
   </si>
   <si>
@@ -1842,99 +1979,6 @@
   </si>
   <si>
     <t>ZWL</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>StockItemID</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>orderId</t>
-  </si>
-  <si>
-    <t>labId</t>
-  </si>
-  <si>
-    <t>batchId</t>
-  </si>
-  <si>
-    <t>dateReceived</t>
-  </si>
-  <si>
-    <t>dateOpened</t>
-  </si>
-  <si>
-    <t>expiryDate</t>
-  </si>
-  <si>
-    <t>disposalDate</t>
-  </si>
-  <si>
-    <t>Stock items</t>
-  </si>
-  <si>
-    <t>Stock item ID</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Order Id</t>
-  </si>
-  <si>
-    <t>Lab Id</t>
-  </si>
-  <si>
-    <t>Batch Id</t>
-  </si>
-  <si>
-    <t>Date Received</t>
-  </si>
-  <si>
-    <t>Date Opened</t>
-  </si>
-  <si>
-    <t>Expiry Date</t>
-  </si>
-  <si>
-    <t>Disposal Date</t>
-  </si>
-  <si>
-    <t>id-001</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>id-002</t>
-  </si>
-  <si>
-    <t>id-003</t>
-  </si>
-  <si>
-    <t>id-004</t>
-  </si>
-  <si>
-    <t>id-005</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>id-006</t>
-  </si>
-  <si>
-    <t>id-007</t>
-  </si>
-  <si>
-    <t>id-008</t>
-  </si>
-  <si>
-    <t>id-009</t>
   </si>
 </sst>
 </file>
@@ -1949,7 +1993,7 @@
     <numFmt numFmtId="168" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2106,6 +2150,25 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2174,7 +2237,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="88">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2451,6 +2514,42 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2489,18 +2588,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2760,7 +2847,7 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3313,1281 +3400,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L200"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2672064777328"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.93927125506073"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.2672064777328"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.21862348178138"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.68421052631579"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.70445344129555"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.82591093117409"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2672064777328"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.37651821862348"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="53" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="69" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>125</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>351</v>
-      </c>
-      <c r="D1" s="70" t="s">
-        <v>352</v>
-      </c>
-      <c r="E1" s="70" t="s">
-        <v>353</v>
-      </c>
-      <c r="F1" s="53" t="s">
-        <v>354</v>
-      </c>
-      <c r="G1" s="71" t="s">
-        <v>355</v>
-      </c>
-      <c r="H1" s="70" t="s">
-        <v>356</v>
-      </c>
-      <c r="I1" s="70" t="s">
-        <v>357</v>
-      </c>
-      <c r="J1" s="70" t="s">
-        <v>358</v>
-      </c>
-      <c r="K1" s="70" t="s">
-        <v>359</v>
-      </c>
-      <c r="L1" s="70"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>184</v>
-      </c>
-      <c r="C2" s="72" t="s">
-        <v>361</v>
-      </c>
-      <c r="D2" s="72" t="s">
-        <v>362</v>
-      </c>
-      <c r="E2" s="73" t="s">
-        <v>363</v>
-      </c>
-      <c r="F2" s="72" t="s">
-        <v>364</v>
-      </c>
-      <c r="G2" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="72" t="s">
-        <v>365</v>
-      </c>
-      <c r="I2" s="72" t="s">
-        <v>366</v>
-      </c>
-      <c r="J2" s="72" t="s">
-        <v>367</v>
-      </c>
-      <c r="K2" s="72" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32" t="s">
-        <v>369</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="72" t="s">
-        <v>370</v>
-      </c>
-      <c r="D3" s="72" t="s">
-        <v>371</v>
-      </c>
-      <c r="E3" s="73" t="s">
-        <v>372</v>
-      </c>
-      <c r="F3" s="72" t="s">
-        <v>373</v>
-      </c>
-      <c r="G3" s="72" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="72" t="s">
-        <v>374</v>
-      </c>
-      <c r="I3" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="72" t="s">
-        <v>375</v>
-      </c>
-      <c r="K3" s="72" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="72" t="s">
-        <v>378</v>
-      </c>
-      <c r="D4" s="72" t="s">
-        <v>379</v>
-      </c>
-      <c r="F4" s="72" t="s">
-        <v>380</v>
-      </c>
-      <c r="G4" s="73"/>
-      <c r="H4" s="72" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="72" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="72" t="s">
-        <v>206</v>
-      </c>
-      <c r="G5" s="73"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="s">
-        <v>382</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>383</v>
-      </c>
-      <c r="G6" s="73"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="72" t="s">
-        <v>201</v>
-      </c>
-      <c r="G7" s="73"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
-        <v>384</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>385</v>
-      </c>
-      <c r="G8" s="73"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="73"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="73"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="73"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="73"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G13" s="73"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="73"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="73"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="73"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="73"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="73"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="73"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="74"/>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-    </row>
-    <row r="21" s="77" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53" t="s">
-        <v>386</v>
-      </c>
-      <c r="B21" s="70" t="s">
-        <v>387</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>388</v>
-      </c>
-      <c r="D21" s="53" t="s">
-        <v>389</v>
-      </c>
-      <c r="E21" s="76" t="s">
-        <v>390</v>
-      </c>
-      <c r="F21" s="53" t="s">
-        <v>391</v>
-      </c>
-      <c r="G21" s="53" t="s">
-        <v>392</v>
-      </c>
-      <c r="H21" s="53" t="s">
-        <v>393</v>
-      </c>
-      <c r="I21" s="53" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="78" t="s">
-        <v>395</v>
-      </c>
-      <c r="B22" s="72" t="s">
-        <v>396</v>
-      </c>
-      <c r="C22" s="72" t="s">
-        <v>397</v>
-      </c>
-      <c r="D22" s="72" t="s">
-        <v>398</v>
-      </c>
-      <c r="E22" s="73" t="s">
-        <v>399</v>
-      </c>
-      <c r="F22" s="72" t="s">
-        <v>400</v>
-      </c>
-      <c r="G22" s="72" t="s">
-        <v>401</v>
-      </c>
-      <c r="H22" s="72" t="s">
-        <v>401</v>
-      </c>
-      <c r="I22" s="72" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="72" t="s">
-        <v>403</v>
-      </c>
-      <c r="C23" s="72" t="s">
-        <v>404</v>
-      </c>
-      <c r="D23" s="72" t="s">
-        <v>405</v>
-      </c>
-      <c r="E23" s="73" t="s">
-        <v>406</v>
-      </c>
-      <c r="F23" s="72" t="s">
-        <v>407</v>
-      </c>
-      <c r="G23" s="72" t="s">
-        <v>408</v>
-      </c>
-      <c r="H23" s="72" t="s">
-        <v>408</v>
-      </c>
-      <c r="I23" s="72" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="72" t="s">
-        <v>410</v>
-      </c>
-      <c r="C24" s="72" t="s">
-        <v>411</v>
-      </c>
-      <c r="D24" s="72" t="s">
-        <v>412</v>
-      </c>
-      <c r="F24" s="72" t="s">
-        <v>413</v>
-      </c>
-      <c r="G24" s="72" t="s">
-        <v>414</v>
-      </c>
-      <c r="H24" s="72" t="s">
-        <v>414</v>
-      </c>
-      <c r="I24" s="72" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="72" t="s">
-        <v>416</v>
-      </c>
-      <c r="C25" s="72" t="s">
-        <v>417</v>
-      </c>
-      <c r="D25" s="72" t="s">
-        <v>418</v>
-      </c>
-      <c r="H25" s="72" t="s">
-        <v>419</v>
-      </c>
-      <c r="I25" s="72" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="72" t="s">
-        <v>421</v>
-      </c>
-      <c r="C26" s="72" t="s">
-        <v>422</v>
-      </c>
-      <c r="H26" s="72" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="72" t="s">
-        <v>424</v>
-      </c>
-      <c r="C27" s="72" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="72" t="s">
-        <v>426</v>
-      </c>
-      <c r="C28" s="72" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="72" t="s">
-        <v>428</v>
-      </c>
-      <c r="C29" s="72" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="72" t="s">
-        <v>430</v>
-      </c>
-      <c r="C30" s="72" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="72" t="s">
-        <v>432</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="72" t="s">
-        <v>434</v>
-      </c>
-      <c r="C32" s="72" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="72" t="s">
-        <v>436</v>
-      </c>
-      <c r="C33" s="72" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="72" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="72" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="72" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="72" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="72" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="72" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="72" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="72" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="72" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="72" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="72" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="72" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="72" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="72" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="72" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="72" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="72" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="72" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="72" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="72" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="72" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="72" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="72" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="72" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="72" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="72" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="72" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="72" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="72" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="72" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="72" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="72" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="72" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="72" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="72" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="72" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="72" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="72" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="72" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="72" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="72" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="72" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="72" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="72" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="72" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="72" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="72" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="72" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="72" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="72" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="72" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="72" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="72" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="72" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="72" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="72" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="72" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="72" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="72" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="72" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="72" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="72" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="72" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="72" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="72" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="72" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="72" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="72" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="72" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="72" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="72" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="72" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="72" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="72" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="72" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="72" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="72" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="72" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="72" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="72" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="72" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="72" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="72" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="72" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="72" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="72" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="72" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="72" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="72" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="72" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="72" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="72" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="72" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="72" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="72" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="72" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="72" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="72" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="72" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="72" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="72" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="72" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="72" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="72" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="72" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="72" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="72" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="72" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="72" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="72" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="72" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="72" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="72" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="72" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="72" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="72" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="72" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="72" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="72" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="72" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="72" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="72" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="72" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="72" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="72" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="72" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="72" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="72" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="72" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="72" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="72" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="72" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="72" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="72" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="72" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="72" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="72" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="72" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="72" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="72" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="72" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="72" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="72" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="72" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="72" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="72" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="72" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="72" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="72" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="72" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="72" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="72" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="72" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="72" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="72" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="72" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="72" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="72" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="72" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="72" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="72" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="72" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="72" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="72" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="72" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="72" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="72" t="s">
-        <v>604</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4607,84 +3423,84 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="79" t="s">
-        <v>605</v>
-      </c>
-      <c r="B1" s="79" t="s">
-        <v>606</v>
-      </c>
-      <c r="C1" s="79" t="s">
+      <c r="A1" s="69" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>352</v>
+      </c>
+      <c r="C1" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="79" t="s">
-        <v>607</v>
-      </c>
-      <c r="E1" s="79" t="s">
+      <c r="D1" s="69" t="s">
+        <v>353</v>
+      </c>
+      <c r="E1" s="69" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="79" t="s">
-        <v>608</v>
-      </c>
-      <c r="G1" s="79" t="s">
-        <v>609</v>
-      </c>
-      <c r="H1" s="79" t="s">
-        <v>610</v>
-      </c>
-      <c r="I1" s="79" t="s">
-        <v>611</v>
-      </c>
-      <c r="J1" s="79" t="s">
-        <v>612</v>
-      </c>
-      <c r="K1" s="79" t="s">
-        <v>613</v>
-      </c>
-      <c r="L1" s="79" t="s">
-        <v>614</v>
+      <c r="F1" s="69" t="s">
+        <v>354</v>
+      </c>
+      <c r="G1" s="69" t="s">
+        <v>355</v>
+      </c>
+      <c r="H1" s="69" t="s">
+        <v>356</v>
+      </c>
+      <c r="I1" s="69" t="s">
+        <v>357</v>
+      </c>
+      <c r="J1" s="69" t="s">
+        <v>358</v>
+      </c>
+      <c r="K1" s="69" t="s">
+        <v>359</v>
+      </c>
+      <c r="L1" s="69" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="80" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="3" s="81" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="81" t="s">
-        <v>605</v>
-      </c>
-      <c r="B3" s="81" t="s">
-        <v>616</v>
-      </c>
-      <c r="C3" s="81" t="s">
+      <c r="A2" s="70" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" s="71" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" s="71" t="s">
+        <v>362</v>
+      </c>
+      <c r="C3" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="81" t="s">
-        <v>617</v>
-      </c>
-      <c r="E3" s="81" t="s">
+      <c r="D3" s="71" t="s">
+        <v>363</v>
+      </c>
+      <c r="E3" s="71" t="s">
         <v>313</v>
       </c>
-      <c r="F3" s="81" t="s">
-        <v>618</v>
-      </c>
-      <c r="G3" s="81" t="s">
-        <v>619</v>
-      </c>
-      <c r="H3" s="81" t="s">
-        <v>620</v>
-      </c>
-      <c r="I3" s="81" t="s">
-        <v>621</v>
-      </c>
-      <c r="J3" s="81" t="s">
-        <v>622</v>
-      </c>
-      <c r="K3" s="81" t="s">
-        <v>623</v>
-      </c>
-      <c r="L3" s="81" t="s">
-        <v>624</v>
+      <c r="F3" s="71" t="s">
+        <v>364</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>365</v>
+      </c>
+      <c r="H3" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="I3" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="J3" s="71" t="s">
+        <v>368</v>
+      </c>
+      <c r="K3" s="71" t="s">
+        <v>369</v>
+      </c>
+      <c r="L3" s="71" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4692,10 +3508,13 @@
         <v>323</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>625</v>
+        <v>371</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>372</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>626</v>
+        <v>373</v>
       </c>
       <c r="E4" s="61" t="n">
         <v>50</v>
@@ -4706,7 +3525,7 @@
         <v>326</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>627</v>
+        <v>374</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>22</v>
@@ -4720,7 +3539,7 @@
         <v>328</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>628</v>
+        <v>375</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>22</v>
@@ -4734,10 +3553,10 @@
         <v>330</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>629</v>
+        <v>376</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>626</v>
+        <v>373</v>
       </c>
       <c r="E7" s="61" t="n">
         <v>100</v>
@@ -4748,10 +3567,10 @@
         <v>332</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>630</v>
+        <v>377</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>631</v>
+        <v>378</v>
       </c>
       <c r="E8" s="61" t="n">
         <v>2</v>
@@ -4762,10 +3581,10 @@
         <v>334</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>632</v>
+        <v>379</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>626</v>
+        <v>373</v>
       </c>
       <c r="E9" s="61" t="n">
         <v>5</v>
@@ -4776,10 +3595,10 @@
         <v>335</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>633</v>
+        <v>380</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>626</v>
+        <v>373</v>
       </c>
       <c r="E10" s="61" t="n">
         <v>123</v>
@@ -4790,10 +3609,10 @@
         <v>341</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>634</v>
+        <v>381</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>631</v>
+        <v>378</v>
       </c>
       <c r="E11" s="61" t="n">
         <v>120</v>
@@ -4804,17 +3623,19 @@
         <v>346</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>635</v>
+        <v>382</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>631</v>
+        <v>378</v>
       </c>
       <c r="E12" s="61" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
@@ -4823,6 +3644,1486 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7408906882591"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8097165991903"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="72" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="72" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>385</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="70" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>308</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="74" t="s">
+        <v>390</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>296</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="74" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4736842105263"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2024291497976"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.0242914979757"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="71" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1" s="71" t="s">
+        <v>386</v>
+      </c>
+      <c r="F1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="70" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="70" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="76" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>395</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>313</v>
+      </c>
+      <c r="F3" s="77"/>
+      <c r="AMJ3" s="77"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="74"/>
+      <c r="B4" s="74" t="s">
+        <v>390</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="74" t="s">
+        <v>390</v>
+      </c>
+      <c r="D5" s="75" t="s">
+        <v>326</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="74" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6" s="75" t="s">
+        <v>328</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="74" t="s">
+        <v>391</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>330</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L200"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2672064777328"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.93927125506073"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.2672064777328"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.21862348178138"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.68421052631579"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.70445344129555"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.82591093117409"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2672064777328"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.37651821862348"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="53" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>397</v>
+      </c>
+      <c r="E1" s="79" t="s">
+        <v>398</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>399</v>
+      </c>
+      <c r="G1" s="80" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1" s="79" t="s">
+        <v>401</v>
+      </c>
+      <c r="I1" s="79" t="s">
+        <v>402</v>
+      </c>
+      <c r="J1" s="79" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1" s="79" t="s">
+        <v>404</v>
+      </c>
+      <c r="L1" s="79"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2" s="82" t="s">
+        <v>408</v>
+      </c>
+      <c r="F2" s="81" t="s">
+        <v>409</v>
+      </c>
+      <c r="G2" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="81" t="s">
+        <v>410</v>
+      </c>
+      <c r="I2" s="81" t="s">
+        <v>411</v>
+      </c>
+      <c r="J2" s="81" t="s">
+        <v>412</v>
+      </c>
+      <c r="K2" s="81" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="32" t="s">
+        <v>414</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="81" t="s">
+        <v>415</v>
+      </c>
+      <c r="D3" s="81" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>417</v>
+      </c>
+      <c r="F3" s="81" t="s">
+        <v>418</v>
+      </c>
+      <c r="G3" s="81" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="81" t="s">
+        <v>419</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="81" t="s">
+        <v>420</v>
+      </c>
+      <c r="K3" s="81" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="81" t="s">
+        <v>423</v>
+      </c>
+      <c r="D4" s="81" t="s">
+        <v>424</v>
+      </c>
+      <c r="F4" s="81" t="s">
+        <v>425</v>
+      </c>
+      <c r="G4" s="82"/>
+      <c r="H4" s="81" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="81" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="81" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" s="82"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="32" t="s">
+        <v>427</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>428</v>
+      </c>
+      <c r="G6" s="82"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="81" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="81" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7" s="82"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="32" t="s">
+        <v>429</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>430</v>
+      </c>
+      <c r="G8" s="82"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G9" s="82"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G10" s="82"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G11" s="82"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G12" s="82"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G13" s="82"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G14" s="82"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G15" s="82"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="82"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G17" s="82"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G18" s="82"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G19" s="82"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="83"/>
+      <c r="K20" s="83"/>
+      <c r="L20" s="83"/>
+    </row>
+    <row r="21" s="86" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="53" t="s">
+        <v>431</v>
+      </c>
+      <c r="B21" s="79" t="s">
+        <v>432</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>433</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>434</v>
+      </c>
+      <c r="E21" s="85" t="s">
+        <v>435</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>436</v>
+      </c>
+      <c r="G21" s="53" t="s">
+        <v>437</v>
+      </c>
+      <c r="H21" s="53" t="s">
+        <v>438</v>
+      </c>
+      <c r="I21" s="53" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="87" t="s">
+        <v>440</v>
+      </c>
+      <c r="B22" s="81" t="s">
+        <v>441</v>
+      </c>
+      <c r="C22" s="81" t="s">
+        <v>442</v>
+      </c>
+      <c r="D22" s="81" t="s">
+        <v>443</v>
+      </c>
+      <c r="E22" s="82" t="s">
+        <v>444</v>
+      </c>
+      <c r="F22" s="81" t="s">
+        <v>445</v>
+      </c>
+      <c r="G22" s="81" t="s">
+        <v>446</v>
+      </c>
+      <c r="H22" s="81" t="s">
+        <v>446</v>
+      </c>
+      <c r="I22" s="81" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="81" t="s">
+        <v>448</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>449</v>
+      </c>
+      <c r="D23" s="81" t="s">
+        <v>450</v>
+      </c>
+      <c r="E23" s="82" t="s">
+        <v>451</v>
+      </c>
+      <c r="F23" s="81" t="s">
+        <v>452</v>
+      </c>
+      <c r="G23" s="81" t="s">
+        <v>453</v>
+      </c>
+      <c r="H23" s="81" t="s">
+        <v>453</v>
+      </c>
+      <c r="I23" s="81" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="81" t="s">
+        <v>455</v>
+      </c>
+      <c r="C24" s="81" t="s">
+        <v>456</v>
+      </c>
+      <c r="D24" s="81" t="s">
+        <v>457</v>
+      </c>
+      <c r="F24" s="81" t="s">
+        <v>458</v>
+      </c>
+      <c r="G24" s="81" t="s">
+        <v>459</v>
+      </c>
+      <c r="H24" s="81" t="s">
+        <v>459</v>
+      </c>
+      <c r="I24" s="81" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="81" t="s">
+        <v>461</v>
+      </c>
+      <c r="C25" s="81" t="s">
+        <v>462</v>
+      </c>
+      <c r="D25" s="81" t="s">
+        <v>463</v>
+      </c>
+      <c r="H25" s="81" t="s">
+        <v>464</v>
+      </c>
+      <c r="I25" s="81" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="81" t="s">
+        <v>466</v>
+      </c>
+      <c r="C26" s="81" t="s">
+        <v>467</v>
+      </c>
+      <c r="H26" s="81" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="81" t="s">
+        <v>469</v>
+      </c>
+      <c r="C27" s="81" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="81" t="s">
+        <v>471</v>
+      </c>
+      <c r="C28" s="81" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="81" t="s">
+        <v>473</v>
+      </c>
+      <c r="C29" s="81" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="81" t="s">
+        <v>475</v>
+      </c>
+      <c r="C30" s="81" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="81" t="s">
+        <v>477</v>
+      </c>
+      <c r="C31" s="81" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="81" t="s">
+        <v>479</v>
+      </c>
+      <c r="C32" s="81" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="81" t="s">
+        <v>481</v>
+      </c>
+      <c r="C33" s="81" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="81" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="81" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="81" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="81" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="81" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="81" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="81" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="81" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="81" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="81" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="81" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="81" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="81" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="81" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="81" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="81" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B50" s="81" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B51" s="81" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="81" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="81" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B54" s="81" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="81" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B56" s="81" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="81" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B58" s="81" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B59" s="81" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B60" s="81" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B61" s="81" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B62" s="81" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B63" s="81" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B64" s="81" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B65" s="81" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B66" s="81" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B67" s="81" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B68" s="81" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B69" s="81" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B70" s="81" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B71" s="81" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B72" s="81" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B73" s="81" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B74" s="81" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B75" s="81" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B76" s="81" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B77" s="81" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B78" s="81" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B79" s="81" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B80" s="81" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B81" s="81" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B82" s="81" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B83" s="81" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B84" s="81" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B85" s="81" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B86" s="81" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B87" s="81" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B88" s="81" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B89" s="81" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B90" s="81" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B91" s="81" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B92" s="81" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B93" s="81" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B94" s="81" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B95" s="81" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B96" s="81" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B97" s="81" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B98" s="81" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B99" s="81" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B100" s="81" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B101" s="81" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B102" s="81" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B103" s="81" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B104" s="81" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B105" s="81" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B106" s="81" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B107" s="81" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B108" s="81" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B109" s="81" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B110" s="81" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B111" s="81" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B112" s="81" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B113" s="81" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B114" s="81" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B115" s="81" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B116" s="81" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B117" s="81" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B118" s="81" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B119" s="81" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B120" s="81" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B121" s="81" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B122" s="81" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B123" s="81" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B124" s="81" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B125" s="81" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B126" s="81" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B127" s="81" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B128" s="81" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B129" s="81" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B130" s="81" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B131" s="81" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B132" s="81" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B133" s="81" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B134" s="81" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B135" s="81" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B136" s="81" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B137" s="81" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B138" s="81" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B139" s="81" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B140" s="81" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B141" s="81" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B142" s="81" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B143" s="81" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B144" s="81" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B145" s="81" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B146" s="81" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B147" s="81" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B148" s="81" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B149" s="81" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B150" s="81" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B151" s="81" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B152" s="81" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B153" s="81" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B154" s="81" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B155" s="81" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B156" s="81" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B157" s="81" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B158" s="81" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B159" s="81" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B160" s="81" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B161" s="81" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B162" s="81" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B163" s="81" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B164" s="81" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B165" s="81" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B166" s="81" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B167" s="81" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B168" s="81" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B169" s="81" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B170" s="81" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B171" s="81" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B172" s="81" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B173" s="81" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B174" s="81" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B175" s="81" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B176" s="81" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B177" s="81" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B178" s="81" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B179" s="81" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B180" s="81" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B181" s="81" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B182" s="81" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B183" s="81" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B184" s="81" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B185" s="81" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B186" s="81" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B187" s="81" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B188" s="81" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B189" s="81" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B190" s="81" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B191" s="81" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B192" s="81" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B193" s="81" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B194" s="81" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B195" s="81" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B196" s="81" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B197" s="81" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B198" s="81" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B199" s="81" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B200" s="81" t="s">
+        <v>649</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Small sticker + bika kit workflow with 3 states: Pending, Assembled and Stored
</commit_message>
<xml_diff>
--- a/bika/sanbi/setupdata/test/test.xlsx
+++ b/bika/sanbi/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="961" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="715" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="863">
   <si>
     <t>Instructions</t>
   </si>
@@ -1718,75 +1718,6 @@
     <t>3ss9515</t>
   </si>
   <si>
-    <t>Spray bottle</t>
-  </si>
-  <si>
-    <t>5822dfd7</t>
-  </si>
-  <si>
-    <t>PET container</t>
-  </si>
-  <si>
-    <t>795ss14</t>
-  </si>
-  <si>
-    <t>Ink cartridge black PGI-7BK</t>
-  </si>
-  <si>
-    <t>da dsfs31</t>
-  </si>
-  <si>
-    <t>Ink cartridge cyan PGI-9C</t>
-  </si>
-  <si>
-    <t>Sulfuric acid</t>
-  </si>
-  <si>
-    <t>7664-93-9</t>
-  </si>
-  <si>
-    <t>323</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>Sulfuric acid and other acids are very corrosive and irritating and cause direct local effects on the skin, eyes, and respiratory and gastrointestinal tracts when there is direct exposure to sufficient concentrations. Breathing sulfuric acid mists can result in tooth erosion and respiratory tract irritation. Drinking concentrated sulfuric acid can burn your mouth and throat, and it can erode a hole in your stomach; it has also resulted in death. If you touch sulfuric acid, it will burn your skin. If you get sulfuric acid in your eyes, it will burn your eyes and cause them to water. The term "burn" used in these sections refers to a chemical burn, not a physical burn resulting from contacting a hot object. People have been blinded by sulfuric acid when it was thrown in their faces.</t>
-  </si>
-  <si>
-    <t>Do not store near combustible materials. Keep container closed when not in use. Store in a cool, dry, well-ventilated area away from incompatible substances. Keep away from water. Corrosives area. Do not store near alkaline substances. Store protected from moisture.</t>
-  </si>
-  <si>
-    <t>Nitric acid</t>
-  </si>
-  <si>
-    <t>7697-37-2</t>
-  </si>
-  <si>
-    <t>3423</t>
-  </si>
-  <si>
-    <t>86 mg/m³ one-hour</t>
-  </si>
-  <si>
-    <t>Concentrated nitric acid and its vapors are highly corrosive to the eyes, skin, and mucous membranes. Dilute solutions cause mild skin irritation and hardening of the epidermis. Contact with concentrated nitric acid stains the skin yellow and produces deep painful burns. Eye contact can cause severe burns and permanent damage. Inhalation of high concentrations can lead to severe respiratory irritation and delayed effects, including pulmonary edema, which may be fatal. Ingestion of nitric acid may result in burning and corrosion of the mouth, throat, and stomach. An oral dose of 10 mL can be fatal in humans.</t>
-  </si>
-  <si>
-    <t>Sodium nitrate</t>
-  </si>
-  <si>
-    <t>7631-99-4</t>
-  </si>
-  <si>
-    <t>3323</t>
-  </si>
-  <si>
-    <t>(1 mg/m3) TWA; (3 mg/m3) STEL</t>
-  </si>
-  <si>
-    <t>Humans are subject to nitrate toxicity, with infants being especially vulnerable to methemoglobinemia due to nitrate metabolizing triglycerides present at higher concentrations than at other stages of development. Methemoglobinemia in infants is known as blue baby syndrome. Although nitrates in drinking water were once thought to be a contributing factor, there are now significant scientific doubts as to whether there is a causal link. Blue baby syndrome is now thought to be the product of a number of factors, which can include any factor that causes gastric upset, such as diarrhoeal infection, protein intolerance, heavy metal toxicity etc., with nitrates playing a minor role.</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -1886,48 +1817,6 @@
     <t>12/02/2014</t>
   </si>
   <si>
-    <t>id-003</t>
-  </si>
-  <si>
-    <t>TF112-1000Q</t>
-  </si>
-  <si>
-    <t>id-004</t>
-  </si>
-  <si>
-    <t>BCBL6953V</t>
-  </si>
-  <si>
-    <t>id-005</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>03/05/2015</t>
-  </si>
-  <si>
-    <t>id-006</t>
-  </si>
-  <si>
-    <t>id-007</t>
-  </si>
-  <si>
-    <t>P2TUB050C</t>
-  </si>
-  <si>
-    <t>id-008</t>
-  </si>
-  <si>
-    <t>G11388</t>
-  </si>
-  <si>
-    <t>id-009</t>
-  </si>
-  <si>
-    <t>25/01/2016</t>
-  </si>
-  <si>
     <t>templateID</t>
   </si>
   <si>
@@ -1949,7 +1838,13 @@
     <t>Template Name</t>
   </si>
   <si>
+    <t>k-001</t>
+  </si>
+  <si>
     <t>DNA Blood sampling kit</t>
+  </si>
+  <si>
+    <t>k-002</t>
   </si>
   <si>
     <t>RNA Blood sampling kit</t>
@@ -2742,7 +2637,7 @@
     <numFmt numFmtId="169" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="170" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2922,6 +2817,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2996,7 +2896,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3369,6 +3269,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5183,7 +5087,7 @@
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -5926,7 +5830,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="true" error="Select a valid instrument from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Instruments' sheet" promptTitle="Select an Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C25" type="list">
-      <formula1>#REF!!$A$1:$A$24</formula1>
+      <formula1>#ref!!$A$1:$A$24</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Not a date" errorTitle="Invalid entry" operator="greaterThan" prompt="After 1 Jan 2012. Expected format is YYYY/MM/DD" promptTitle="Please enter a date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:F25" type="date">
@@ -6082,7 +5986,7 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6311,32 +6215,16 @@
       <c r="U5" s="65"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60" t="s">
-        <v>561</v>
-      </c>
-      <c r="C6" s="61" t="s">
-        <v>527</v>
-      </c>
-      <c r="D6" s="61" t="s">
-        <v>301</v>
-      </c>
+      <c r="A6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
       <c r="E6" s="62"/>
-      <c r="F6" s="62" t="s">
-        <v>562</v>
-      </c>
-      <c r="G6" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="59" t="n">
-        <v>50</v>
-      </c>
+      <c r="F6" s="62"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="59"/>
       <c r="I6" s="63"/>
-      <c r="J6" s="64" t="n">
-        <v>12.11</v>
-      </c>
-      <c r="K6" s="64" t="n">
-        <v>12.11</v>
-      </c>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
       <c r="L6" s="59"/>
       <c r="M6" s="59"/>
       <c r="N6" s="64"/>
@@ -6348,32 +6236,16 @@
       <c r="U6" s="65"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="60" t="s">
-        <v>563</v>
-      </c>
-      <c r="C7" s="61" t="s">
-        <v>527</v>
-      </c>
-      <c r="D7" s="61" t="s">
-        <v>301</v>
-      </c>
+      <c r="A7" s="60"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
       <c r="E7" s="62"/>
-      <c r="F7" s="62" t="s">
-        <v>564</v>
-      </c>
-      <c r="G7" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="59" t="n">
-        <v>100</v>
-      </c>
+      <c r="F7" s="62"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="59"/>
       <c r="I7" s="63"/>
-      <c r="J7" s="64" t="n">
-        <v>12.11</v>
-      </c>
-      <c r="K7" s="64" t="n">
-        <v>12.11</v>
-      </c>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
       <c r="L7" s="59"/>
       <c r="M7" s="59"/>
       <c r="N7" s="64"/>
@@ -6385,33 +6257,17 @@
       <c r="U7" s="65"/>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="60" t="s">
-        <v>565</v>
-      </c>
+      <c r="A8" s="60"/>
       <c r="B8" s="21"/>
-      <c r="C8" s="61" t="s">
-        <v>536</v>
-      </c>
-      <c r="D8" s="61" t="s">
-        <v>303</v>
-      </c>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="62"/>
-      <c r="F8" s="62" t="s">
-        <v>566</v>
-      </c>
-      <c r="G8" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="59" t="n">
-        <v>2</v>
-      </c>
+      <c r="F8" s="62"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="59"/>
       <c r="I8" s="63"/>
-      <c r="J8" s="64" t="n">
-        <v>12.11</v>
-      </c>
-      <c r="K8" s="64" t="n">
-        <v>53.11</v>
-      </c>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
       <c r="L8" s="59"/>
       <c r="M8" s="59"/>
       <c r="N8" s="64"/>
@@ -6423,33 +6279,17 @@
       <c r="U8" s="65"/>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="60" t="s">
-        <v>567</v>
-      </c>
+      <c r="A9" s="60"/>
       <c r="B9" s="21"/>
-      <c r="C9" s="61" t="s">
-        <v>536</v>
-      </c>
-      <c r="D9" s="61" t="s">
-        <v>303</v>
-      </c>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="62"/>
-      <c r="F9" s="62" t="n">
-        <v>2323</v>
-      </c>
-      <c r="G9" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="59" t="n">
-        <v>5</v>
-      </c>
+      <c r="F9" s="62"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="59"/>
       <c r="I9" s="63"/>
-      <c r="J9" s="64" t="n">
-        <v>12.11</v>
-      </c>
-      <c r="K9" s="64" t="n">
-        <v>12.11</v>
-      </c>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
       <c r="L9" s="59"/>
       <c r="M9" s="59"/>
       <c r="N9" s="64"/>
@@ -6461,44 +6301,20 @@
       <c r="U9" s="65"/>
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
-        <v>568</v>
-      </c>
+      <c r="A10" s="21"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="61" t="s">
-        <v>539</v>
-      </c>
-      <c r="D10" s="61" t="s">
-        <v>301</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>569</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>570</v>
-      </c>
-      <c r="G10" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="59" t="n">
-        <v>123</v>
-      </c>
-      <c r="I10" s="63" t="s">
-        <v>571</v>
-      </c>
-      <c r="J10" s="64" t="n">
-        <v>12.11</v>
-      </c>
-      <c r="K10" s="64" t="n">
-        <v>12.11</v>
-      </c>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
       <c r="L10" s="59"/>
-      <c r="M10" s="84" t="s">
-        <v>572</v>
-      </c>
-      <c r="N10" s="64" t="s">
-        <v>573</v>
-      </c>
+      <c r="M10" s="84"/>
+      <c r="N10" s="64"/>
       <c r="P10" s="21"/>
       <c r="Q10" s="40"/>
       <c r="R10" s="40"/>
@@ -6506,42 +6322,20 @@
       <c r="T10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
-        <v>574</v>
-      </c>
+      <c r="A11" s="21"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="61" t="s">
-        <v>539</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>301</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>575</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>576</v>
-      </c>
-      <c r="G11" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="59" t="n">
-        <v>120</v>
-      </c>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="59"/>
       <c r="I11" s="63"/>
       <c r="J11" s="64"/>
-      <c r="K11" s="64" t="n">
-        <v>12.11</v>
-      </c>
-      <c r="L11" s="85" t="s">
-        <v>577</v>
-      </c>
-      <c r="M11" s="84" t="s">
-        <v>578</v>
-      </c>
-      <c r="N11" s="64" t="s">
-        <v>573</v>
-      </c>
+      <c r="K11" s="64"/>
+      <c r="L11" s="85"/>
+      <c r="M11" s="84"/>
+      <c r="N11" s="64"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="40"/>
       <c r="R11" s="40"/>
@@ -6549,39 +6343,19 @@
       <c r="T11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
-        <v>579</v>
-      </c>
+      <c r="A12" s="21"/>
       <c r="B12" s="21"/>
-      <c r="C12" s="61" t="s">
-        <v>539</v>
-      </c>
-      <c r="D12" s="61" t="s">
-        <v>301</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>580</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>581</v>
-      </c>
-      <c r="G12" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="59" t="n">
-        <v>10</v>
-      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="59"/>
       <c r="I12" s="59"/>
       <c r="J12" s="64"/>
-      <c r="K12" s="64" t="n">
-        <v>12.11</v>
-      </c>
-      <c r="L12" s="85" t="s">
-        <v>582</v>
-      </c>
-      <c r="M12" s="64" t="s">
-        <v>583</v>
-      </c>
+      <c r="K12" s="64"/>
+      <c r="L12" s="85"/>
+      <c r="M12" s="64"/>
       <c r="N12" s="64"/>
       <c r="P12" s="21"/>
       <c r="Q12" s="40"/>
@@ -6603,7 +6377,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L4:N10 N11:N12 M12:N12" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L4:N10 N11 M12:N12" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6635,10 +6409,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6662,69 +6436,69 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="87" t="s">
-        <v>584</v>
+        <v>561</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>585</v>
+        <v>562</v>
       </c>
       <c r="C1" s="87" t="s">
         <v>42</v>
       </c>
       <c r="D1" s="87" t="s">
-        <v>586</v>
+        <v>563</v>
       </c>
       <c r="E1" s="87" t="s">
-        <v>587</v>
+        <v>564</v>
       </c>
       <c r="F1" s="87" t="s">
         <v>546</v>
       </c>
       <c r="G1" s="87" t="s">
-        <v>588</v>
+        <v>565</v>
       </c>
       <c r="H1" s="87" t="s">
-        <v>589</v>
+        <v>566</v>
       </c>
       <c r="I1" s="87" t="s">
-        <v>590</v>
+        <v>567</v>
       </c>
       <c r="J1" s="87" t="s">
-        <v>591</v>
+        <v>568</v>
       </c>
       <c r="K1" s="87" t="s">
-        <v>592</v>
+        <v>569</v>
       </c>
       <c r="L1" s="87" t="s">
-        <v>593</v>
+        <v>570</v>
       </c>
       <c r="M1" s="87" t="s">
-        <v>594</v>
+        <v>571</v>
       </c>
       <c r="N1" s="87" t="s">
-        <v>595</v>
+        <v>572</v>
       </c>
       <c r="O1" s="87" t="s">
-        <v>596</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="42" t="s">
-        <v>597</v>
+        <v>574</v>
       </c>
       <c r="D2" s="0"/>
     </row>
     <row r="3" s="88" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="88" t="s">
-        <v>584</v>
+        <v>561</v>
       </c>
       <c r="B3" s="88" t="s">
-        <v>598</v>
+        <v>575</v>
       </c>
       <c r="C3" s="88" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="88" t="s">
-        <v>599</v>
+        <v>576</v>
       </c>
       <c r="E3" s="88" t="s">
         <v>345</v>
@@ -6733,31 +6507,31 @@
         <v>546</v>
       </c>
       <c r="G3" s="88" t="s">
-        <v>600</v>
+        <v>577</v>
       </c>
       <c r="H3" s="88" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="I3" s="88" t="s">
-        <v>602</v>
+        <v>579</v>
       </c>
       <c r="J3" s="88" t="s">
-        <v>603</v>
+        <v>580</v>
       </c>
       <c r="K3" s="88" t="s">
-        <v>604</v>
+        <v>581</v>
       </c>
       <c r="L3" s="88" t="s">
-        <v>605</v>
+        <v>582</v>
       </c>
       <c r="M3" s="88" t="s">
-        <v>606</v>
+        <v>583</v>
       </c>
       <c r="N3" s="88" t="s">
-        <v>607</v>
+        <v>584</v>
       </c>
       <c r="O3" s="88" t="s">
-        <v>608</v>
+        <v>585</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6765,22 +6539,22 @@
         <v>556</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>609</v>
+        <v>586</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>610</v>
+        <v>587</v>
       </c>
       <c r="D4" s="86" t="s">
-        <v>611</v>
+        <v>588</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>612</v>
+        <v>589</v>
       </c>
       <c r="F4" s="59" t="n">
         <v>50</v>
       </c>
       <c r="J4" s="89" t="s">
-        <v>613</v>
+        <v>590</v>
       </c>
       <c r="K4" s="89" t="n">
         <v>1</v>
@@ -6791,10 +6565,10 @@
         <v>559</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>614</v>
+        <v>591</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>615</v>
+        <v>592</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>22</v>
@@ -6803,166 +6577,15 @@
         <v>25</v>
       </c>
       <c r="J5" s="89" t="s">
-        <v>616</v>
+        <v>593</v>
       </c>
       <c r="K5" s="89" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60" t="s">
-        <v>561</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>617</v>
-      </c>
-      <c r="D6" s="86" t="s">
-        <v>618</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="59" t="n">
-        <v>50</v>
-      </c>
-      <c r="J6" s="89"/>
-      <c r="K6" s="89" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="60" t="s">
-        <v>563</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>619</v>
-      </c>
-      <c r="D7" s="86" t="s">
-        <v>620</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="F7" s="59" t="n">
-        <v>100</v>
-      </c>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="60" t="s">
-        <v>565</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>621</v>
-      </c>
-      <c r="D8" s="86" t="n">
-        <v>301746</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="F8" s="59" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" s="89" t="s">
-        <v>623</v>
-      </c>
-      <c r="K8" s="89" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="60" t="s">
-        <v>567</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>624</v>
-      </c>
-      <c r="D9" s="86" t="n">
-        <v>301747</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="F9" s="59" t="n">
-        <v>5</v>
-      </c>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
-        <v>568</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>625</v>
-      </c>
-      <c r="D10" s="86" t="s">
-        <v>626</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="F10" s="59" t="n">
-        <v>123</v>
-      </c>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
-        <v>574</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>627</v>
-      </c>
-      <c r="D11" s="86" t="s">
-        <v>628</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="F11" s="59" t="n">
-        <v>120</v>
-      </c>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
-        <v>579</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>629</v>
-      </c>
-      <c r="D12" s="86" t="n">
-        <v>368815</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="F12" s="59" t="n">
-        <v>10</v>
-      </c>
-      <c r="J12" s="89" t="s">
-        <v>630</v>
-      </c>
-      <c r="K12" s="89" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="greaterThan" prompt="Whole number" promptTitle="Quantity" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4:F12" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThan" prompt="Whole number" promptTitle="Quantity" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4:F5" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6985,7 +6608,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6999,29 +6622,29 @@
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>631</v>
+        <v>594</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>632</v>
+        <v>595</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>633</v>
+        <v>596</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>634</v>
+        <v>597</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="42" t="s">
-        <v>635</v>
+        <v>598</v>
       </c>
     </row>
     <row r="3" s="43" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="43" t="s">
-        <v>636</v>
+        <v>599</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>637</v>
+        <v>600</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>542</v>
@@ -7031,8 +6654,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>601</v>
+      </c>
       <c r="B4" s="90" t="s">
-        <v>638</v>
+        <v>602</v>
       </c>
       <c r="C4" s="91" t="s">
         <v>524</v>
@@ -7042,8 +6668,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>603</v>
+      </c>
       <c r="B5" s="90" t="s">
-        <v>639</v>
+        <v>604</v>
       </c>
       <c r="C5" s="90" t="s">
         <v>539</v>
@@ -7068,10 +6697,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:7"/>
+  <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7087,42 +6716,42 @@
   <sheetData>
     <row r="1" s="88" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="88" t="s">
-        <v>631</v>
+        <v>594</v>
       </c>
       <c r="B1" s="88" t="s">
-        <v>632</v>
+        <v>595</v>
       </c>
       <c r="C1" s="88" t="s">
-        <v>640</v>
+        <v>605</v>
       </c>
       <c r="D1" s="88" t="s">
-        <v>641</v>
+        <v>606</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>634</v>
+        <v>597</v>
       </c>
       <c r="F1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="42" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="42" t="s">
-        <v>635</v>
+        <v>598</v>
       </c>
       <c r="F2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="92" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="92" t="s">
-        <v>636</v>
+        <v>599</v>
       </c>
       <c r="B3" s="92" t="s">
-        <v>637</v>
+        <v>600</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>642</v>
+        <v>607</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>643</v>
+        <v>608</v>
       </c>
       <c r="E3" s="92" t="s">
         <v>546</v>
@@ -7133,7 +6762,7 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="90"/>
       <c r="B4" s="90" t="s">
-        <v>638</v>
+        <v>602</v>
       </c>
       <c r="D4" s="91" t="s">
         <v>556</v>
@@ -7144,7 +6773,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="90" t="s">
-        <v>638</v>
+        <v>602</v>
       </c>
       <c r="D5" s="91" t="s">
         <v>559</v>
@@ -7155,24 +6784,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="90" t="s">
-        <v>639</v>
-      </c>
-      <c r="D6" s="91" t="s">
-        <v>561</v>
+        <v>604</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>559</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="90" t="s">
-        <v>639</v>
-      </c>
-      <c r="D7" s="91" t="s">
-        <v>563</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7211,1239 +6829,1239 @@
   </cols>
   <sheetData>
     <row r="1" s="53" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="94" t="s">
-        <v>644</v>
-      </c>
-      <c r="D1" s="94" t="s">
-        <v>645</v>
-      </c>
-      <c r="E1" s="94" t="s">
-        <v>646</v>
+      <c r="C1" s="95" t="s">
+        <v>609</v>
+      </c>
+      <c r="D1" s="95" t="s">
+        <v>610</v>
+      </c>
+      <c r="E1" s="95" t="s">
+        <v>611</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>647</v>
-      </c>
-      <c r="G1" s="95" t="s">
-        <v>648</v>
-      </c>
-      <c r="H1" s="94" t="s">
-        <v>649</v>
-      </c>
-      <c r="I1" s="94" t="s">
-        <v>650</v>
-      </c>
-      <c r="J1" s="94" t="s">
-        <v>651</v>
-      </c>
-      <c r="K1" s="94" t="s">
-        <v>652</v>
-      </c>
-      <c r="L1" s="94"/>
+        <v>612</v>
+      </c>
+      <c r="G1" s="96" t="s">
+        <v>613</v>
+      </c>
+      <c r="H1" s="95" t="s">
+        <v>614</v>
+      </c>
+      <c r="I1" s="95" t="s">
+        <v>615</v>
+      </c>
+      <c r="J1" s="95" t="s">
+        <v>616</v>
+      </c>
+      <c r="K1" s="95" t="s">
+        <v>617</v>
+      </c>
+      <c r="L1" s="95"/>
     </row>
     <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>653</v>
+        <v>618</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="96" t="s">
-        <v>654</v>
-      </c>
-      <c r="D2" s="96" t="s">
-        <v>655</v>
-      </c>
-      <c r="E2" s="97" t="s">
-        <v>656</v>
-      </c>
-      <c r="F2" s="96" t="s">
-        <v>657</v>
-      </c>
-      <c r="G2" s="96" t="n">
+      <c r="C2" s="97" t="s">
+        <v>619</v>
+      </c>
+      <c r="D2" s="97" t="s">
+        <v>620</v>
+      </c>
+      <c r="E2" s="98" t="s">
+        <v>621</v>
+      </c>
+      <c r="F2" s="97" t="s">
+        <v>622</v>
+      </c>
+      <c r="G2" s="97" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="96" t="s">
-        <v>658</v>
-      </c>
-      <c r="I2" s="96" t="s">
-        <v>659</v>
-      </c>
-      <c r="J2" s="96" t="s">
-        <v>660</v>
-      </c>
-      <c r="K2" s="96" t="s">
-        <v>661</v>
+      <c r="H2" s="97" t="s">
+        <v>623</v>
+      </c>
+      <c r="I2" s="97" t="s">
+        <v>624</v>
+      </c>
+      <c r="J2" s="97" t="s">
+        <v>625</v>
+      </c>
+      <c r="K2" s="97" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>662</v>
+        <v>627</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="96" t="s">
-        <v>663</v>
-      </c>
-      <c r="D3" s="96" t="s">
-        <v>664</v>
-      </c>
-      <c r="E3" s="97" t="s">
-        <v>665</v>
-      </c>
-      <c r="F3" s="96" t="s">
-        <v>666</v>
-      </c>
-      <c r="G3" s="96" t="n">
+      <c r="C3" s="97" t="s">
+        <v>628</v>
+      </c>
+      <c r="D3" s="97" t="s">
+        <v>629</v>
+      </c>
+      <c r="E3" s="98" t="s">
+        <v>630</v>
+      </c>
+      <c r="F3" s="97" t="s">
+        <v>631</v>
+      </c>
+      <c r="G3" s="97" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="96" t="s">
-        <v>667</v>
-      </c>
-      <c r="I3" s="96" t="s">
+      <c r="H3" s="97" t="s">
+        <v>632</v>
+      </c>
+      <c r="I3" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="96" t="s">
-        <v>668</v>
-      </c>
-      <c r="K3" s="96" t="s">
-        <v>669</v>
+      <c r="J3" s="97" t="s">
+        <v>633</v>
+      </c>
+      <c r="K3" s="97" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>670</v>
+        <v>635</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="C4" s="96" t="s">
-        <v>671</v>
-      </c>
-      <c r="D4" s="96" t="s">
-        <v>672</v>
-      </c>
-      <c r="F4" s="96" t="s">
-        <v>673</v>
-      </c>
-      <c r="G4" s="97"/>
-      <c r="H4" s="96" t="s">
-        <v>674</v>
+      <c r="C4" s="97" t="s">
+        <v>636</v>
+      </c>
+      <c r="D4" s="97" t="s">
+        <v>637</v>
+      </c>
+      <c r="F4" s="97" t="s">
+        <v>638</v>
+      </c>
+      <c r="G4" s="98"/>
+      <c r="H4" s="97" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="97" t="s">
         <v>204</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="97" t="s">
         <v>206</v>
       </c>
-      <c r="G5" s="97"/>
+      <c r="G5" s="98"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>675</v>
+        <v>640</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>676</v>
-      </c>
-      <c r="G6" s="97"/>
+        <v>641</v>
+      </c>
+      <c r="G6" s="98"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="97" t="s">
         <v>199</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="97" t="s">
         <v>201</v>
       </c>
-      <c r="G7" s="97"/>
+      <c r="G7" s="98"/>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
+        <v>642</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>643</v>
+      </c>
+      <c r="G8" s="98"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G9" s="98"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G10" s="98"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G11" s="98"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G12" s="98"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G13" s="98"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G14" s="98"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G15" s="98"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="98"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G17" s="98"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G18" s="98"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G19" s="98"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="99"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="99"/>
+      <c r="L20" s="99"/>
+    </row>
+    <row r="21" s="102" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="53" t="s">
+        <v>644</v>
+      </c>
+      <c r="B21" s="95" t="s">
+        <v>645</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>646</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>647</v>
+      </c>
+      <c r="E21" s="101" t="s">
+        <v>648</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>649</v>
+      </c>
+      <c r="G21" s="53" t="s">
+        <v>650</v>
+      </c>
+      <c r="H21" s="53" t="s">
+        <v>651</v>
+      </c>
+      <c r="I21" s="53" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="103" t="s">
+        <v>653</v>
+      </c>
+      <c r="B22" s="97" t="s">
+        <v>654</v>
+      </c>
+      <c r="C22" s="97" t="s">
+        <v>655</v>
+      </c>
+      <c r="D22" s="97" t="s">
+        <v>656</v>
+      </c>
+      <c r="E22" s="98" t="s">
+        <v>657</v>
+      </c>
+      <c r="F22" s="97" t="s">
+        <v>658</v>
+      </c>
+      <c r="G22" s="97" t="s">
+        <v>659</v>
+      </c>
+      <c r="H22" s="97" t="s">
+        <v>659</v>
+      </c>
+      <c r="I22" s="97" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="97" t="s">
+        <v>661</v>
+      </c>
+      <c r="C23" s="97" t="s">
+        <v>662</v>
+      </c>
+      <c r="D23" s="97" t="s">
+        <v>663</v>
+      </c>
+      <c r="E23" s="98" t="s">
+        <v>664</v>
+      </c>
+      <c r="F23" s="97" t="s">
+        <v>665</v>
+      </c>
+      <c r="G23" s="97" t="s">
+        <v>666</v>
+      </c>
+      <c r="H23" s="97" t="s">
+        <v>666</v>
+      </c>
+      <c r="I23" s="97" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="97" t="s">
+        <v>668</v>
+      </c>
+      <c r="C24" s="97" t="s">
+        <v>669</v>
+      </c>
+      <c r="D24" s="97" t="s">
+        <v>670</v>
+      </c>
+      <c r="F24" s="97" t="s">
+        <v>671</v>
+      </c>
+      <c r="G24" s="97" t="s">
+        <v>672</v>
+      </c>
+      <c r="H24" s="97" t="s">
+        <v>672</v>
+      </c>
+      <c r="I24" s="97" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="97" t="s">
+        <v>674</v>
+      </c>
+      <c r="C25" s="97" t="s">
+        <v>675</v>
+      </c>
+      <c r="D25" s="97" t="s">
+        <v>676</v>
+      </c>
+      <c r="H25" s="97" t="s">
         <v>677</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="I25" s="97" t="s">
         <v>678</v>
       </c>
-      <c r="G8" s="97"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="97"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="97"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="97"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="97"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G13" s="97"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="97"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="97"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="97"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="97"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="97"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="97"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="98"/>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="98"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
-    </row>
-    <row r="21" s="101" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="97" t="s">
         <v>679</v>
       </c>
-      <c r="B21" s="94" t="s">
+      <c r="C26" s="97" t="s">
         <v>680</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="H26" s="97" t="s">
         <v>681</v>
       </c>
-      <c r="D21" s="53" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="97" t="s">
         <v>682</v>
       </c>
-      <c r="E21" s="100" t="s">
+      <c r="C27" s="97" t="s">
         <v>683</v>
       </c>
-      <c r="F21" s="53" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="97" t="s">
         <v>684</v>
       </c>
-      <c r="G21" s="53" t="s">
+      <c r="C28" s="97" t="s">
         <v>685</v>
       </c>
-      <c r="H21" s="53" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="97" t="s">
         <v>686</v>
       </c>
-      <c r="I21" s="53" t="s">
+      <c r="C29" s="97" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="102" t="s">
+    <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="97" t="s">
         <v>688</v>
       </c>
-      <c r="B22" s="96" t="s">
+      <c r="C30" s="97" t="s">
         <v>689</v>
       </c>
-      <c r="C22" s="96" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="97" t="s">
         <v>690</v>
       </c>
-      <c r="D22" s="96" t="s">
+      <c r="C31" s="97" t="s">
         <v>691</v>
       </c>
-      <c r="E22" s="97" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="97" t="s">
         <v>692</v>
       </c>
-      <c r="F22" s="96" t="s">
+      <c r="C32" s="97" t="s">
         <v>693</v>
       </c>
-      <c r="G22" s="96" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="97" t="s">
         <v>694</v>
       </c>
-      <c r="H22" s="96" t="s">
-        <v>694</v>
-      </c>
-      <c r="I22" s="96" t="s">
+      <c r="C33" s="97" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="96" t="s">
+    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="97" t="s">
         <v>696</v>
       </c>
-      <c r="C23" s="96" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="97" t="s">
         <v>697</v>
       </c>
-      <c r="D23" s="96" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="97" t="s">
         <v>698</v>
       </c>
-      <c r="E23" s="97" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="97" t="s">
         <v>699</v>
       </c>
-      <c r="F23" s="96" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="97" t="s">
         <v>700</v>
       </c>
-      <c r="G23" s="96" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="97" t="s">
         <v>701</v>
       </c>
-      <c r="H23" s="96" t="s">
-        <v>701</v>
-      </c>
-      <c r="I23" s="96" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="97" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="96" t="s">
+    <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="97" t="s">
         <v>703</v>
       </c>
-      <c r="C24" s="96" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="97" t="s">
         <v>704</v>
       </c>
-      <c r="D24" s="96" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="97" t="s">
         <v>705</v>
       </c>
-      <c r="F24" s="96" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="97" t="s">
         <v>706</v>
       </c>
-      <c r="G24" s="96" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="97" t="s">
         <v>707</v>
       </c>
-      <c r="H24" s="96" t="s">
-        <v>707</v>
-      </c>
-      <c r="I24" s="96" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="97" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="96" t="s">
+    <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="97" t="s">
         <v>709</v>
       </c>
-      <c r="C25" s="96" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="97" t="s">
         <v>710</v>
       </c>
-      <c r="D25" s="96" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="97" t="s">
         <v>711</v>
       </c>
-      <c r="H25" s="96" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B50" s="97" t="s">
         <v>712</v>
       </c>
-      <c r="I25" s="96" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B51" s="97" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="96" t="s">
+    <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="97" t="s">
         <v>714</v>
       </c>
-      <c r="C26" s="96" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="97" t="s">
         <v>715</v>
       </c>
-      <c r="H26" s="96" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B54" s="97" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="96" t="s">
+    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="97" t="s">
         <v>717</v>
       </c>
-      <c r="C27" s="96" t="s">
+    </row>
+    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B56" s="97" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="96" t="s">
+    <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="97" t="s">
         <v>719</v>
       </c>
-      <c r="C28" s="96" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B58" s="97" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="96" t="s">
+    <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B59" s="97" t="s">
         <v>721</v>
       </c>
-      <c r="C29" s="96" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B60" s="97" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="96" t="s">
+    <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B61" s="97" t="s">
         <v>723</v>
       </c>
-      <c r="C30" s="96" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B62" s="97" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="96" t="s">
+    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B63" s="97" t="s">
         <v>725</v>
       </c>
-      <c r="C31" s="96" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B64" s="97" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="96" t="s">
+    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B65" s="97" t="s">
         <v>727</v>
       </c>
-      <c r="C32" s="96" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B66" s="97" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="96" t="s">
+    <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B67" s="97" t="s">
         <v>729</v>
       </c>
-      <c r="C33" s="96" t="s">
+    </row>
+    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B68" s="97" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="96" t="s">
+    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B69" s="97" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="96" t="s">
+    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B70" s="97" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="96" t="s">
+    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B71" s="97" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="96" t="s">
+    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B72" s="97" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="96" t="s">
+    <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B73" s="97" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="96" t="s">
+    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B74" s="97" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="96" t="s">
+    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B75" s="97" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="96" t="s">
+    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B76" s="97" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="96" t="s">
+    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B77" s="97" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="96" t="s">
+    <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B78" s="97" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="96" t="s">
+    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B79" s="97" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="96" t="s">
+    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B80" s="97" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="96" t="s">
+    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B81" s="97" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="96" t="s">
+    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B82" s="97" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="96" t="s">
+    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B83" s="97" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="96" t="s">
+    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B84" s="97" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="96" t="s">
+    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B85" s="97" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="96" t="s">
+    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B86" s="97" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="96" t="s">
+    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B87" s="97" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="96" t="s">
+    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B88" s="97" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="96" t="s">
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B89" s="97" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="96" t="s">
+    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B90" s="97" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="96" t="s">
+    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B91" s="97" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="96" t="s">
+    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B92" s="97" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="96" t="s">
+    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B93" s="97" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="96" t="s">
+    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B94" s="97" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="96" t="s">
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B95" s="97" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="96" t="s">
+    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B96" s="97" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="96" t="s">
+    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B97" s="97" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="96" t="s">
+    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B98" s="97" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="96" t="s">
+    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B99" s="97" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="96" t="s">
+    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B100" s="97" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="96" t="s">
+    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B101" s="97" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="96" t="s">
+    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B102" s="97" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="96" t="s">
+    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B103" s="97" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="96" t="s">
+    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B104" s="97" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="96" t="s">
+    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B105" s="97" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="96" t="s">
+    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B106" s="97" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="96" t="s">
+    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B107" s="97" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="96" t="s">
+    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B108" s="97" t="s">
         <v>770</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="96" t="s">
+    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B109" s="97" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="96" t="s">
+    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B110" s="97" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="96" t="s">
+    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B111" s="97" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="96" t="s">
+    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B112" s="97" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="96" t="s">
+    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B113" s="97" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="96" t="s">
+    <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B114" s="97" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="96" t="s">
+    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B115" s="97" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="96" t="s">
+    <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B116" s="97" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="96" t="s">
+    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B117" s="97" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="96" t="s">
+    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B118" s="97" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="96" t="s">
+    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B119" s="97" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="96" t="s">
+    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B120" s="97" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="96" t="s">
+    <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B121" s="97" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="96" t="s">
+    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B122" s="97" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="96" t="s">
+    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B123" s="97" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="96" t="s">
+    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B124" s="97" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="96" t="s">
+    <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B125" s="97" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="96" t="s">
+    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B126" s="97" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="96" t="s">
+    <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B127" s="97" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="96" t="s">
+    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B128" s="97" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="96" t="s">
+    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B129" s="97" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="96" t="s">
+    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B130" s="97" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="96" t="s">
+    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B131" s="97" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="96" t="s">
+    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B132" s="97" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="96" t="s">
+    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B133" s="97" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="96" t="s">
+    <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B134" s="97" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="96" t="s">
+    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B135" s="97" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="96" t="s">
+    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B136" s="97" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="96" t="s">
+    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B137" s="97" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="96" t="s">
+    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B138" s="97" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="96" t="s">
+    <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B139" s="97" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="96" t="s">
+    <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B140" s="97" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="96" t="s">
+    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B141" s="97" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="96" t="s">
+    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B142" s="97" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="96" t="s">
+    <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B143" s="97" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="96" t="s">
+    <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B144" s="97" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="96" t="s">
+    <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B145" s="97" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="96" t="s">
+    <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B146" s="97" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="96" t="s">
+    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B147" s="97" t="s">
         <v>809</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="96" t="s">
+    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B148" s="97" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="96" t="s">
+    <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B149" s="97" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="96" t="s">
+    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B150" s="97" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="96" t="s">
+    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B151" s="97" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="96" t="s">
+    <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B152" s="97" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="96" t="s">
+    <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B153" s="97" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="96" t="s">
+    <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B154" s="97" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="96" t="s">
+    <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B155" s="97" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="96" t="s">
+    <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B156" s="97" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="96" t="s">
+    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B157" s="97" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="96" t="s">
+    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B158" s="97" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="96" t="s">
+    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B159" s="97" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="96" t="s">
+    <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B160" s="97" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="96" t="s">
+    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B161" s="97" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="96" t="s">
+    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B162" s="97" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="96" t="s">
+    <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B163" s="97" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="96" t="s">
+    <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B164" s="97" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="96" t="s">
+    <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B165" s="97" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="96" t="s">
+    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B166" s="97" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="96" t="s">
+    <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B167" s="97" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="96" t="s">
+    <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B168" s="97" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="96" t="s">
+    <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B169" s="97" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="96" t="s">
+    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B170" s="97" t="s">
         <v>832</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="96" t="s">
+    <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B171" s="97" t="s">
         <v>833</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="96" t="s">
+    <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B172" s="97" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="96" t="s">
+    <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B173" s="97" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="96" t="s">
+    <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B174" s="97" t="s">
         <v>836</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="96" t="s">
+    <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B175" s="97" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="96" t="s">
+    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B176" s="97" t="s">
         <v>838</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="96" t="s">
+    <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B177" s="97" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="96" t="s">
+    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B178" s="97" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="96" t="s">
+    <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B179" s="97" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="96" t="s">
+    <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B180" s="97" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="96" t="s">
+    <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B181" s="97" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="96" t="s">
+    <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B182" s="97" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="96" t="s">
+    <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B183" s="97" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="96" t="s">
+    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B184" s="97" t="s">
         <v>846</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="96" t="s">
+    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B185" s="97" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="96" t="s">
+    <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B186" s="97" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="96" t="s">
+    <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B187" s="97" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="96" t="s">
+    <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B188" s="97" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="96" t="s">
+    <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B189" s="97" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="96" t="s">
+    <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B190" s="97" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="96" t="s">
+    <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B191" s="97" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="96" t="s">
+    <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B192" s="97" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="96" t="s">
+    <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B193" s="97" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="96" t="s">
+    <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B194" s="97" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="96" t="s">
+    <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B195" s="97" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="96" t="s">
+    <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B196" s="97" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="96" t="s">
+    <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B197" s="97" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="96" t="s">
+    <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B198" s="97" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="96" t="s">
+    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B199" s="97" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="96" t="s">
+    <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B200" s="97" t="s">
         <v>862</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="96" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="96" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="96" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="96" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="96" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="96" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="96" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="96" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="96" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="96" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="96" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="96" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="96" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="96" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="96" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="96" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="96" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="96" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="96" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="96" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="96" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="96" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="96" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="96" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="96" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="96" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="96" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="96" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="96" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="96" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="96" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="96" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="96" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="96" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="96" t="s">
-        <v>897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow manager users to create shipments
</commit_message>
<xml_diff>
--- a/bika/sanbi/setupdata/test/test.xlsx
+++ b/bika/sanbi/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="791" firstSheet="0" activeTab="34"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="395" firstSheet="0" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -14844,7 +14844,7 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -14960,8 +14960,8 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -15165,6 +15165,12 @@
       <c r="C11" s="0" t="s">
         <v>935</v>
       </c>
+      <c r="D11" s="180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="180" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="104" t="s">
@@ -15176,6 +15182,12 @@
       <c r="C12" s="0" t="s">
         <v>937</v>
       </c>
+      <c r="D12" s="180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="180" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="104" t="s">
@@ -15187,6 +15199,12 @@
       <c r="C13" s="0" t="s">
         <v>939</v>
       </c>
+      <c r="D13" s="180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="180" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="104" t="s">
@@ -15197,6 +15215,12 @@
       </c>
       <c r="C14" s="0" t="s">
         <v>941</v>
+      </c>
+      <c r="D14" s="180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="180" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15467,7 +15491,7 @@
   </sheetPr>
   <dimension ref="A1:AE14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Y14" activeCellId="0" sqref="Y14"/>
     </sheetView>
   </sheetViews>

</xml_diff>